<commit_message>
Runtime changes, Scenario load processing
</commit_message>
<xml_diff>
--- a/TUFLOWFV/site_processing/peel/Scenarios_Spreadsheets/HAB OXY Crit.xlsx
+++ b/TUFLOWFV/site_processing/peel/Scenarios_Spreadsheets/HAB OXY Crit.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\aed_matlab_modeltools\TUFLOWFV\site_processing\peel\Scenarios_Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2018\aed_matlab_modeltools\TUFLOWFV\site_processing\peel\Scenarios_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA29FDC-8720-4246-A2CE-5F91DE5612AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1EE5B552-DBF6-414A-A7CF-2D6AD5841C40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="29">
   <si>
     <t>Region</t>
   </si>
@@ -113,11 +112,17 @@
   <si>
     <t>Bottom Oxy &lt; 4</t>
   </si>
+  <si>
+    <t>CL 1 &gt; 0.5</t>
+  </si>
+  <si>
+    <t>CL 2 &gt; 0.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -260,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -281,6 +286,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,39 +600,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFF59CC-70DE-4512-96D5-A7C53B52114A}">
-  <dimension ref="A1:AF42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47:U47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="1"/>
+    <col min="12" max="12" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="1"/>
-    <col min="23" max="23" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1796875" style="1"/>
+    <col min="23" max="23" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="32" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="33" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
@@ -665,7 +671,7 @@
       <c r="AE1" s="15"/>
       <c r="AF1" s="15"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -757,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -849,7 +855,7 @@
         <v>28.456499999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -941,7 +947,7 @@
         <v>4.4321000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>6.8470000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>41.0762</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>8.2635000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>1.3224</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>0.61950000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1493,7 +1499,7 @@
         <v>9.0226000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>69.946600000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>11.225</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>16.832899999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>73.243300000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -1953,7 +1959,7 @@
         <v>27.4437</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>13.1905</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>11.118499999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>22.2499</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>10.1653</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>5.6268000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>4.0679999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>9.3071000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>39.1143</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>19</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>25.400700000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>19</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>27.039899999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>46.081899999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>18.9389</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>8.1570999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
@@ -3241,7 +3247,7 @@
         <v>9.5260999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>26.8536</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>21</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>1.3966000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>8.3500000000000005E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>21</v>
       </c>
@@ -3609,7 +3615,7 @@
         <v>1.3429</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>21</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>4.2107999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>22</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>22</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>1.1361000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>3.9043999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>22</v>
       </c>
@@ -4069,7 +4075,7 @@
         <v>7.7965</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>23</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>7.0838999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>23</v>
       </c>
@@ -4253,7 +4259,7 @@
         <v>3.3289</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>23</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>5.7183000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>23</v>
       </c>
@@ -4437,11 +4443,2579 @@
         <v>9.0297000000000001</v>
       </c>
     </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="M46" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O47" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P47" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R47" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="S47" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="T47" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="U47" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M48" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N48" s="1">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0</v>
+      </c>
+      <c r="R48" s="1">
+        <v>0</v>
+      </c>
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
+        <v>0</v>
+      </c>
+      <c r="U48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0</v>
+      </c>
+      <c r="O49" s="1">
+        <v>0</v>
+      </c>
+      <c r="P49" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>0</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0</v>
+      </c>
+      <c r="S49" s="1">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1">
+        <v>0</v>
+      </c>
+      <c r="U49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N50" s="1">
+        <v>0</v>
+      </c>
+      <c r="O50" s="1">
+        <v>0</v>
+      </c>
+      <c r="P50" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <v>0</v>
+      </c>
+      <c r="U50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N51" s="1">
+        <v>0</v>
+      </c>
+      <c r="O51" s="1">
+        <v>0</v>
+      </c>
+      <c r="P51" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>0</v>
+      </c>
+      <c r="R51" s="1">
+        <v>0</v>
+      </c>
+      <c r="S51" s="1">
+        <v>0</v>
+      </c>
+      <c r="T51" s="1">
+        <v>0</v>
+      </c>
+      <c r="U51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N52" s="1">
+        <v>0</v>
+      </c>
+      <c r="O52" s="1">
+        <v>0</v>
+      </c>
+      <c r="P52" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <v>0</v>
+      </c>
+      <c r="U52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+      <c r="L53" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N53" s="1">
+        <v>0</v>
+      </c>
+      <c r="O53" s="1">
+        <v>0</v>
+      </c>
+      <c r="P53" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="R53" s="1">
+        <v>0</v>
+      </c>
+      <c r="S53" s="1">
+        <v>0</v>
+      </c>
+      <c r="T53" s="1">
+        <v>0</v>
+      </c>
+      <c r="U53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0</v>
+      </c>
+      <c r="L54" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M54" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N54" s="1">
+        <v>0</v>
+      </c>
+      <c r="O54" s="1">
+        <v>0</v>
+      </c>
+      <c r="P54" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+      <c r="R54" s="1">
+        <v>0</v>
+      </c>
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+      <c r="T54" s="1">
+        <v>0</v>
+      </c>
+      <c r="U54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M55" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
+      </c>
+      <c r="O55" s="1">
+        <v>0</v>
+      </c>
+      <c r="P55" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>0</v>
+      </c>
+      <c r="R55" s="1">
+        <v>0</v>
+      </c>
+      <c r="S55" s="1">
+        <v>0</v>
+      </c>
+      <c r="T55" s="1">
+        <v>0</v>
+      </c>
+      <c r="U55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N56" s="1">
+        <v>0</v>
+      </c>
+      <c r="O56" s="1">
+        <v>0</v>
+      </c>
+      <c r="P56" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>0</v>
+      </c>
+      <c r="R56" s="1">
+        <v>0</v>
+      </c>
+      <c r="S56" s="1">
+        <v>0</v>
+      </c>
+      <c r="T56" s="1">
+        <v>0</v>
+      </c>
+      <c r="U56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N57" s="1">
+        <v>0</v>
+      </c>
+      <c r="O57" s="1">
+        <v>0</v>
+      </c>
+      <c r="P57" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>0</v>
+      </c>
+      <c r="R57" s="1">
+        <v>0</v>
+      </c>
+      <c r="S57" s="1">
+        <v>0</v>
+      </c>
+      <c r="T57" s="1">
+        <v>0</v>
+      </c>
+      <c r="U57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+      <c r="L58" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M58" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N58" s="1">
+        <v>0</v>
+      </c>
+      <c r="O58" s="1">
+        <v>0</v>
+      </c>
+      <c r="P58" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>0</v>
+      </c>
+      <c r="R58" s="1">
+        <v>0</v>
+      </c>
+      <c r="S58" s="1">
+        <v>0</v>
+      </c>
+      <c r="T58" s="1">
+        <v>0</v>
+      </c>
+      <c r="U58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N59" s="1">
+        <v>0</v>
+      </c>
+      <c r="O59" s="1">
+        <v>0</v>
+      </c>
+      <c r="P59" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>0</v>
+      </c>
+      <c r="R59" s="1">
+        <v>0</v>
+      </c>
+      <c r="S59" s="1">
+        <v>0</v>
+      </c>
+      <c r="T59" s="1">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M60" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N60" s="1">
+        <v>0.19489999999999999</v>
+      </c>
+      <c r="O60" s="1">
+        <v>0.2616</v>
+      </c>
+      <c r="P60" s="1">
+        <v>0.90110000000000001</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>0.75329999999999997</v>
+      </c>
+      <c r="R60" s="1">
+        <v>0.4955</v>
+      </c>
+      <c r="S60" s="1">
+        <v>0.75470000000000004</v>
+      </c>
+      <c r="T60" s="1">
+        <v>0.96660000000000001</v>
+      </c>
+      <c r="U60" s="1">
+        <v>0.79139999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="L61" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M61" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N61" s="1">
+        <v>0</v>
+      </c>
+      <c r="O61" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="R61" s="1">
+        <v>0</v>
+      </c>
+      <c r="S61" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="T61" s="1">
+        <v>0</v>
+      </c>
+      <c r="U61" s="1">
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="1">
+        <v>6.6566999999999998</v>
+      </c>
+      <c r="D62" s="1">
+        <v>4.5427</v>
+      </c>
+      <c r="E62" s="1">
+        <v>8.6305999999999994</v>
+      </c>
+      <c r="F62" s="1">
+        <v>5.6635</v>
+      </c>
+      <c r="G62" s="1">
+        <v>8.3667999999999996</v>
+      </c>
+      <c r="H62" s="1">
+        <v>5.6684999999999999</v>
+      </c>
+      <c r="I62" s="1">
+        <v>8.8819999999999997</v>
+      </c>
+      <c r="J62" s="1">
+        <v>5.8632</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M62" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N62" s="1">
+        <v>9.6641999999999992</v>
+      </c>
+      <c r="O62" s="1">
+        <v>15.2803</v>
+      </c>
+      <c r="P62" s="1">
+        <v>11.5334</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>15.4925</v>
+      </c>
+      <c r="R62" s="1">
+        <v>11.9869</v>
+      </c>
+      <c r="S62" s="1">
+        <v>15.522</v>
+      </c>
+      <c r="T62" s="1">
+        <v>11.4773</v>
+      </c>
+      <c r="U62" s="1">
+        <v>15.411</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="1">
+        <v>4.2621000000000002</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>6.1821999999999999</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>5.8460999999999999</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>6.2382999999999997</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+      <c r="L63" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N63" s="1">
+        <v>9.5512999999999995</v>
+      </c>
+      <c r="O63" s="1">
+        <v>2.8607</v>
+      </c>
+      <c r="P63" s="1">
+        <v>14.100099999999999</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>3.6535000000000002</v>
+      </c>
+      <c r="R63" s="1">
+        <v>13.4855</v>
+      </c>
+      <c r="S63" s="1">
+        <v>3.6669999999999998</v>
+      </c>
+      <c r="T63" s="1">
+        <v>14.2751</v>
+      </c>
+      <c r="U63" s="1">
+        <v>4.0946999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M64" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N64" s="1">
+        <v>0.57809999999999995</v>
+      </c>
+      <c r="O64" s="1">
+        <v>0.71630000000000005</v>
+      </c>
+      <c r="P64" s="1">
+        <v>2.3613</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>1.792</v>
+      </c>
+      <c r="R64" s="1">
+        <v>1.1137999999999999</v>
+      </c>
+      <c r="S64" s="1">
+        <v>1.8013999999999999</v>
+      </c>
+      <c r="T64" s="1">
+        <v>2.6080999999999999</v>
+      </c>
+      <c r="U64" s="1">
+        <v>1.8879999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+      <c r="L65" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M65" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N65" s="1">
+        <v>0</v>
+      </c>
+      <c r="O65" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="P65" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="R65" s="1">
+        <v>0</v>
+      </c>
+      <c r="S65" s="1">
+        <v>6.2100000000000002E-2</v>
+      </c>
+      <c r="T65" s="1">
+        <v>0</v>
+      </c>
+      <c r="U65" s="1">
+        <v>5.7200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="1">
+        <v>25.7637</v>
+      </c>
+      <c r="D66" s="1">
+        <v>13.3279</v>
+      </c>
+      <c r="E66" s="1">
+        <v>24.419699999999999</v>
+      </c>
+      <c r="F66" s="1">
+        <v>16.734000000000002</v>
+      </c>
+      <c r="G66" s="1">
+        <v>23.740100000000002</v>
+      </c>
+      <c r="H66" s="1">
+        <v>16.748000000000001</v>
+      </c>
+      <c r="I66" s="1">
+        <v>25.057099999999998</v>
+      </c>
+      <c r="J66" s="1">
+        <v>17.3185</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M66" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N66" s="1">
+        <v>51.017699999999998</v>
+      </c>
+      <c r="O66" s="1">
+        <v>76.501099999999994</v>
+      </c>
+      <c r="P66" s="1">
+        <v>53.176499999999997</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>78.336100000000002</v>
+      </c>
+      <c r="R66" s="1">
+        <v>54.87</v>
+      </c>
+      <c r="S66" s="1">
+        <v>78.414599999999993</v>
+      </c>
+      <c r="T66" s="1">
+        <v>52.598399999999998</v>
+      </c>
+      <c r="U66" s="1">
+        <v>77.867800000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="1">
+        <v>16.627700000000001</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>17.655999999999999</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>16.868600000000001</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>18.161799999999999</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M67" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N67" s="1">
+        <v>61.585500000000003</v>
+      </c>
+      <c r="O67" s="1">
+        <v>22.0992</v>
+      </c>
+      <c r="P67" s="1">
+        <v>80.649600000000007</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>28.0656</v>
+      </c>
+      <c r="R67" s="1">
+        <v>78.083600000000004</v>
+      </c>
+      <c r="S67" s="1">
+        <v>28.137</v>
+      </c>
+      <c r="T67" s="1">
+        <v>81.629499999999993</v>
+      </c>
+      <c r="U67" s="1">
+        <v>30.7956</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0</v>
+      </c>
+      <c r="L68" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N68" s="1">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="O68" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="P68" s="1">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="R68" s="1">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="S68" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="T68" s="1">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="U68" s="1">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0</v>
+      </c>
+      <c r="L69" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M69" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N69" s="1">
+        <v>0</v>
+      </c>
+      <c r="O69" s="1">
+        <v>0</v>
+      </c>
+      <c r="P69" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="R69" s="1">
+        <v>0</v>
+      </c>
+      <c r="S69" s="1">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="T69" s="1">
+        <v>0</v>
+      </c>
+      <c r="U69" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="1">
+        <v>11.996499999999999</v>
+      </c>
+      <c r="D70" s="1">
+        <v>6.8068</v>
+      </c>
+      <c r="E70" s="1">
+        <v>18.0076</v>
+      </c>
+      <c r="F70" s="1">
+        <v>10.4421</v>
+      </c>
+      <c r="G70" s="1">
+        <v>17.141500000000001</v>
+      </c>
+      <c r="H70" s="1">
+        <v>10.4495</v>
+      </c>
+      <c r="I70" s="1">
+        <v>18.864999999999998</v>
+      </c>
+      <c r="J70" s="1">
+        <v>11.115399999999999</v>
+      </c>
+      <c r="L70" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M70" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N70" s="1">
+        <v>37.106299999999997</v>
+      </c>
+      <c r="O70" s="1">
+        <v>52.056600000000003</v>
+      </c>
+      <c r="P70" s="1">
+        <v>45.403500000000001</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>54.264600000000002</v>
+      </c>
+      <c r="R70" s="1">
+        <v>46.934699999999999</v>
+      </c>
+      <c r="S70" s="1">
+        <v>54.334099999999999</v>
+      </c>
+      <c r="T70" s="1">
+        <v>46.094200000000001</v>
+      </c>
+      <c r="U70" s="1">
+        <v>54.350099999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3.7366999999999999</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>12.3087</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <v>9.3796999999999997</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>13.2563</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N71" s="1">
+        <v>21.323699999999999</v>
+      </c>
+      <c r="O71" s="1">
+        <v>7.8090999999999999</v>
+      </c>
+      <c r="P71" s="1">
+        <v>47.726399999999998</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>9.5032999999999994</v>
+      </c>
+      <c r="R71" s="1">
+        <v>45.495699999999999</v>
+      </c>
+      <c r="S71" s="1">
+        <v>9.5525000000000002</v>
+      </c>
+      <c r="T71" s="1">
+        <v>48.480400000000003</v>
+      </c>
+      <c r="U71" s="1">
+        <v>10.0723</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+      <c r="L72" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M72" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N72" s="1">
+        <v>2.2153</v>
+      </c>
+      <c r="O72" s="1">
+        <v>2.6432000000000002</v>
+      </c>
+      <c r="P72" s="1">
+        <v>4.5949999999999998</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>4.4775</v>
+      </c>
+      <c r="R72" s="1">
+        <v>3.0844</v>
+      </c>
+      <c r="S72" s="1">
+        <v>4.4911000000000003</v>
+      </c>
+      <c r="T72" s="1">
+        <v>4.7544000000000004</v>
+      </c>
+      <c r="U72" s="1">
+        <v>4.5738000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="L73" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M73" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N73" s="1">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="O73" s="1">
+        <v>4.3E-3</v>
+      </c>
+      <c r="P73" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="R73" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="S73" s="1">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="T73" s="1">
+        <v>0</v>
+      </c>
+      <c r="U73" s="1">
+        <v>5.6500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="1">
+        <v>17.6983</v>
+      </c>
+      <c r="D74" s="1">
+        <v>9.4975000000000005</v>
+      </c>
+      <c r="E74" s="1">
+        <v>20.897500000000001</v>
+      </c>
+      <c r="F74" s="1">
+        <v>13.0427</v>
+      </c>
+      <c r="G74" s="1">
+        <v>20.020499999999998</v>
+      </c>
+      <c r="H74" s="1">
+        <v>13.0467</v>
+      </c>
+      <c r="I74" s="1">
+        <v>21.579899999999999</v>
+      </c>
+      <c r="J74" s="1">
+        <v>13.711399999999999</v>
+      </c>
+      <c r="L74" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M74" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N74" s="1">
+        <v>48.874600000000001</v>
+      </c>
+      <c r="O74" s="1">
+        <v>60.569499999999998</v>
+      </c>
+      <c r="P74" s="1">
+        <v>48.925199999999997</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>63.395899999999997</v>
+      </c>
+      <c r="R74" s="1">
+        <v>50.033799999999999</v>
+      </c>
+      <c r="S74" s="1">
+        <v>63.469099999999997</v>
+      </c>
+      <c r="T74" s="1">
+        <v>48.867600000000003</v>
+      </c>
+      <c r="U74" s="1">
+        <v>63.517400000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="1">
+        <v>17.479299999999999</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1">
+        <v>20.228899999999999</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>19.075800000000001</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>20.837</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0</v>
+      </c>
+      <c r="L75" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M75" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N75" s="1">
+        <v>52.330599999999997</v>
+      </c>
+      <c r="O75" s="1">
+        <v>38.962000000000003</v>
+      </c>
+      <c r="P75" s="1">
+        <v>62.470599999999997</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>46.072499999999998</v>
+      </c>
+      <c r="R75" s="1">
+        <v>62.0428</v>
+      </c>
+      <c r="S75" s="1">
+        <v>46.241700000000002</v>
+      </c>
+      <c r="T75" s="1">
+        <v>63.146000000000001</v>
+      </c>
+      <c r="U75" s="1">
+        <v>48.062199999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0</v>
+      </c>
+      <c r="J76" s="1">
+        <v>0</v>
+      </c>
+      <c r="L76" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M76" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N76" s="1">
+        <v>10.8508</v>
+      </c>
+      <c r="O76" s="1">
+        <v>11.1767</v>
+      </c>
+      <c r="P76" s="1">
+        <v>13.3508</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>14.1617</v>
+      </c>
+      <c r="R76" s="1">
+        <v>11.7004</v>
+      </c>
+      <c r="S76" s="1">
+        <v>14.162699999999999</v>
+      </c>
+      <c r="T76" s="1">
+        <v>13.4132</v>
+      </c>
+      <c r="U76" s="1">
+        <v>14.2134</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1">
+        <v>0</v>
+      </c>
+      <c r="L77" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M77" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N77" s="1">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="O77" s="1">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0.1143</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0.186</v>
+      </c>
+      <c r="R77" s="1">
+        <v>0.1401</v>
+      </c>
+      <c r="S77" s="1">
+        <v>0.186</v>
+      </c>
+      <c r="T77" s="1">
+        <v>0.1138</v>
+      </c>
+      <c r="U77" s="1">
+        <v>0.19470000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.60709999999999997</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.15079999999999999</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0.23880000000000001</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0.63270000000000004</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.2382</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.76239999999999997</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0.2487</v>
+      </c>
+      <c r="L78" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M78" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N78" s="1">
+        <v>36.334299999999999</v>
+      </c>
+      <c r="O78" s="1">
+        <v>41.260800000000003</v>
+      </c>
+      <c r="P78" s="1">
+        <v>41.217599999999997</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>44.666899999999998</v>
+      </c>
+      <c r="R78" s="1">
+        <v>41.475999999999999</v>
+      </c>
+      <c r="S78" s="1">
+        <v>44.671900000000001</v>
+      </c>
+      <c r="T78" s="1">
+        <v>41.186700000000002</v>
+      </c>
+      <c r="U78" s="1">
+        <v>44.677999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.6956</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.37240000000000001</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0</v>
+      </c>
+      <c r="L79" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M79" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N79" s="1">
+        <v>55.736699999999999</v>
+      </c>
+      <c r="O79" s="1">
+        <v>56.790100000000002</v>
+      </c>
+      <c r="P79" s="1">
+        <v>59.265799999999999</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>58.047199999999997</v>
+      </c>
+      <c r="R79" s="1">
+        <v>59.076799999999999</v>
+      </c>
+      <c r="S79" s="1">
+        <v>57.855699999999999</v>
+      </c>
+      <c r="T79" s="1">
+        <v>59.122300000000003</v>
+      </c>
+      <c r="U79" s="1">
+        <v>57.953099999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="L80" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M80" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N80" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="O80" s="1">
+        <v>2.2936999999999999</v>
+      </c>
+      <c r="P80" s="1">
+        <v>3.9773999999999998</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>3.9304000000000001</v>
+      </c>
+      <c r="R80" s="1">
+        <v>2.4881000000000002</v>
+      </c>
+      <c r="S80" s="1">
+        <v>3.6067999999999998</v>
+      </c>
+      <c r="T80" s="1">
+        <v>3.7021000000000002</v>
+      </c>
+      <c r="U80" s="1">
+        <v>3.6126999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0</v>
+      </c>
+      <c r="J81" s="1">
+        <v>0</v>
+      </c>
+      <c r="L81" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M81" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N81" s="1">
+        <v>0</v>
+      </c>
+      <c r="O81" s="1">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="P81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="R81" s="1">
+        <v>0</v>
+      </c>
+      <c r="S81" s="1">
+        <v>0.1608</v>
+      </c>
+      <c r="T81" s="1">
+        <v>0</v>
+      </c>
+      <c r="U81" s="1">
+        <v>0.1555</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="1">
+        <v>5.0366999999999997</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3.2155999999999998</v>
+      </c>
+      <c r="E82" s="1">
+        <v>6.3749000000000002</v>
+      </c>
+      <c r="F82" s="1">
+        <v>4.3297999999999996</v>
+      </c>
+      <c r="G82" s="1">
+        <v>5.7462999999999997</v>
+      </c>
+      <c r="H82" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="I82" s="1">
+        <v>6.3666999999999998</v>
+      </c>
+      <c r="J82" s="1">
+        <v>4.3556999999999997</v>
+      </c>
+      <c r="L82" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M82" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N82" s="1">
+        <v>59.155500000000004</v>
+      </c>
+      <c r="O82" s="1">
+        <v>63.607700000000001</v>
+      </c>
+      <c r="P82" s="1">
+        <v>60.424300000000002</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>67.063599999999994</v>
+      </c>
+      <c r="R82" s="1">
+        <v>61.039299999999997</v>
+      </c>
+      <c r="S82" s="1">
+        <v>66.635199999999998</v>
+      </c>
+      <c r="T82" s="1">
+        <v>59.978200000000001</v>
+      </c>
+      <c r="U82" s="1">
+        <v>66.627200000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+      <c r="L83" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M83" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N83" s="1">
+        <v>51.196899999999999</v>
+      </c>
+      <c r="O83" s="1">
+        <v>45.724400000000003</v>
+      </c>
+      <c r="P83" s="1">
+        <v>70.959199999999996</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>49.750100000000003</v>
+      </c>
+      <c r="R83" s="1">
+        <v>63.987299999999998</v>
+      </c>
+      <c r="S83" s="1">
+        <v>49.259700000000002</v>
+      </c>
+      <c r="T83" s="1">
+        <v>70.506900000000002</v>
+      </c>
+      <c r="U83" s="1">
+        <v>49.519399999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+      <c r="L84" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M84" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N84" s="1">
+        <v>0.1236</v>
+      </c>
+      <c r="O84" s="1">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="P84" s="1">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>0.18379999999999999</v>
+      </c>
+      <c r="R84" s="1">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="S84" s="1">
+        <v>0.1825</v>
+      </c>
+      <c r="T84" s="1">
+        <v>0.30049999999999999</v>
+      </c>
+      <c r="U84" s="1">
+        <v>0.1827</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+      <c r="L85" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M85" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N85" s="1">
+        <v>0</v>
+      </c>
+      <c r="O85" s="1">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="P85" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="1">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="R85" s="1">
+        <v>0</v>
+      </c>
+      <c r="S85" s="1">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="T85" s="1">
+        <v>0</v>
+      </c>
+      <c r="U85" s="1">
+        <v>2.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="1">
+        <v>19.789200000000001</v>
+      </c>
+      <c r="D86" s="1">
+        <v>19.463699999999999</v>
+      </c>
+      <c r="E86" s="1">
+        <v>25.187999999999999</v>
+      </c>
+      <c r="F86" s="1">
+        <v>22.996200000000002</v>
+      </c>
+      <c r="G86" s="1">
+        <v>24.636099999999999</v>
+      </c>
+      <c r="H86" s="1">
+        <v>22.933700000000002</v>
+      </c>
+      <c r="I86" s="1">
+        <v>25.2087</v>
+      </c>
+      <c r="J86" s="1">
+        <v>23.0594</v>
+      </c>
+      <c r="L86" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M86" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N86" s="1">
+        <v>49.1051</v>
+      </c>
+      <c r="O86" s="1">
+        <v>69.195999999999998</v>
+      </c>
+      <c r="P86" s="1">
+        <v>62.072000000000003</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>73.124099999999999</v>
+      </c>
+      <c r="R86" s="1">
+        <v>63.107300000000002</v>
+      </c>
+      <c r="S86" s="1">
+        <v>73.005499999999998</v>
+      </c>
+      <c r="T86" s="1">
+        <v>61.941400000000002</v>
+      </c>
+      <c r="U86" s="1">
+        <v>72.801100000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="1">
+        <v>3.5346000000000002</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.76090000000000002</v>
+      </c>
+      <c r="E87" s="1">
+        <v>5.4996999999999998</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="G87" s="1">
+        <v>3.6802999999999999</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0.95530000000000004</v>
+      </c>
+      <c r="I87" s="1">
+        <v>5.5048000000000004</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="L87" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M87" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N87" s="1">
+        <v>41.376600000000003</v>
+      </c>
+      <c r="O87" s="1">
+        <v>48.701900000000002</v>
+      </c>
+      <c r="P87" s="1">
+        <v>81.530100000000004</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>52.900399999999998</v>
+      </c>
+      <c r="R87" s="1">
+        <v>64.625299999999996</v>
+      </c>
+      <c r="S87" s="1">
+        <v>52.440399999999997</v>
+      </c>
+      <c r="T87" s="1">
+        <v>81.999399999999994</v>
+      </c>
+      <c r="U87" s="1">
+        <v>52.690199999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="M1:U1"/>
     <mergeCell ref="X1:AF1"/>
+    <mergeCell ref="B46:J46"/>
+    <mergeCell ref="M46:U46"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:J42">
     <cfRule type="colorScale" priority="2">
@@ -4468,6 +7042,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>